<commit_message>
Adicionando comentários no Scraping e Começando análise dos dados: plotando os valores dos modelos agrupados por marca
</commit_message>
<xml_diff>
--- a/Dados Tabela Fipe.xlsx
+++ b/Dados Tabela Fipe.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K473"/>
+  <dimension ref="A1:K481"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25506,6 +25506,430 @@
         </is>
       </c>
     </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>R$ 29.620,00</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>GM - Chevrolet</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>Astra 2.0/ CD/ GLS 2.0 MPFI 16V 3p</t>
+        </is>
+      </c>
+      <c r="D474" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E474" t="inlineStr">
+        <is>
+          <t>Gasolina</t>
+        </is>
+      </c>
+      <c r="F474" t="inlineStr">
+        <is>
+          <t>004169-6</t>
+        </is>
+      </c>
+      <c r="G474" t="inlineStr">
+        <is>
+          <t xml:space="preserve">fevereiro de 2001 </t>
+        </is>
+      </c>
+      <c r="H474" t="inlineStr">
+        <is>
+          <t>pjmjmk4kqmc</t>
+        </is>
+      </c>
+      <c r="I474" t="n">
+        <v>1</v>
+      </c>
+      <c r="J474" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="K474" t="inlineStr">
+        <is>
+          <t>sexta-feira, 2 de fevereiro de 2024 17:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>R$ 29.620,00</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>GM - Chevrolet</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>Astra 2.0/ CD/ GLS 2.0 MPFI 16V 3p</t>
+        </is>
+      </c>
+      <c r="D475" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E475" t="inlineStr">
+        <is>
+          <t>Gasolina</t>
+        </is>
+      </c>
+      <c r="F475" t="inlineStr">
+        <is>
+          <t>004169-6</t>
+        </is>
+      </c>
+      <c r="G475" t="inlineStr">
+        <is>
+          <t xml:space="preserve">fevereiro de 2001 </t>
+        </is>
+      </c>
+      <c r="H475" t="inlineStr">
+        <is>
+          <t>pjmjmk4kqmc</t>
+        </is>
+      </c>
+      <c r="I475" t="n">
+        <v>1</v>
+      </c>
+      <c r="J475" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="K475" t="inlineStr">
+        <is>
+          <t>sexta-feira, 2 de fevereiro de 2024 18:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>R$ 29.620,00</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>GM - Chevrolet</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>Astra 2.0/ CD/ GLS 2.0 MPFI 16V 3p</t>
+        </is>
+      </c>
+      <c r="D476" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E476" t="inlineStr">
+        <is>
+          <t>Gasolina</t>
+        </is>
+      </c>
+      <c r="F476" t="inlineStr">
+        <is>
+          <t>004169-6</t>
+        </is>
+      </c>
+      <c r="G476" t="inlineStr">
+        <is>
+          <t xml:space="preserve">fevereiro de 2001 </t>
+        </is>
+      </c>
+      <c r="H476" t="inlineStr">
+        <is>
+          <t>pjmjmk4kqmc</t>
+        </is>
+      </c>
+      <c r="I476" t="n">
+        <v>1</v>
+      </c>
+      <c r="J476" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="K476" t="inlineStr">
+        <is>
+          <t>sexta-feira, 2 de fevereiro de 2024 18:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>R$ 13.629,00</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>GM - Chevrolet</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>Celta 1.0/Super/N.Piq.1.0 MPFi VHC 8V 3p</t>
+        </is>
+      </c>
+      <c r="D477" t="n">
+        <v>2001</v>
+      </c>
+      <c r="E477" t="inlineStr">
+        <is>
+          <t>Gasolina</t>
+        </is>
+      </c>
+      <c r="F477" t="inlineStr">
+        <is>
+          <t>004202-1</t>
+        </is>
+      </c>
+      <c r="G477" t="inlineStr">
+        <is>
+          <t xml:space="preserve">fevereiro de 2001 </t>
+        </is>
+      </c>
+      <c r="H477" t="inlineStr">
+        <is>
+          <t>hg3826wm6jc</t>
+        </is>
+      </c>
+      <c r="I477" t="n">
+        <v>1</v>
+      </c>
+      <c r="J477" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="K477" t="inlineStr">
+        <is>
+          <t>sexta-feira, 2 de fevereiro de 2024 18:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>R$ 29.620,00</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>GM - Chevrolet</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>Astra 2.0/ CD/ GLS 2.0 MPFI 16V 3p</t>
+        </is>
+      </c>
+      <c r="D478" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E478" t="inlineStr">
+        <is>
+          <t>Gasolina</t>
+        </is>
+      </c>
+      <c r="F478" t="inlineStr">
+        <is>
+          <t>004169-6</t>
+        </is>
+      </c>
+      <c r="G478" t="inlineStr">
+        <is>
+          <t xml:space="preserve">fevereiro de 2001 </t>
+        </is>
+      </c>
+      <c r="H478" t="inlineStr">
+        <is>
+          <t>pjmjmk4kqmc</t>
+        </is>
+      </c>
+      <c r="I478" t="n">
+        <v>1</v>
+      </c>
+      <c r="J478" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="K478" t="inlineStr">
+        <is>
+          <t>sexta-feira, 2 de fevereiro de 2024 18:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>R$ 29.620,00</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>GM - Chevrolet</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>Astra 2.0/ CD/ GLS 2.0 MPFI 16V 3p</t>
+        </is>
+      </c>
+      <c r="D479" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E479" t="inlineStr">
+        <is>
+          <t>Gasolina</t>
+        </is>
+      </c>
+      <c r="F479" t="inlineStr">
+        <is>
+          <t>004169-6</t>
+        </is>
+      </c>
+      <c r="G479" t="inlineStr">
+        <is>
+          <t xml:space="preserve">fevereiro de 2001 </t>
+        </is>
+      </c>
+      <c r="H479" t="inlineStr">
+        <is>
+          <t>pjmjmk4kqmc</t>
+        </is>
+      </c>
+      <c r="I479" t="n">
+        <v>1</v>
+      </c>
+      <c r="J479" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="K479" t="inlineStr">
+        <is>
+          <t>sexta-feira, 2 de fevereiro de 2024 18:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>R$ 13.629,00</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>GM - Chevrolet</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>Celta 1.0/Super/N.Piq.1.0 MPFi VHC 8V 3p</t>
+        </is>
+      </c>
+      <c r="D480" t="n">
+        <v>2001</v>
+      </c>
+      <c r="E480" t="inlineStr">
+        <is>
+          <t>Gasolina</t>
+        </is>
+      </c>
+      <c r="F480" t="inlineStr">
+        <is>
+          <t>004202-1</t>
+        </is>
+      </c>
+      <c r="G480" t="inlineStr">
+        <is>
+          <t xml:space="preserve">fevereiro de 2001 </t>
+        </is>
+      </c>
+      <c r="H480" t="inlineStr">
+        <is>
+          <t>hg3826wm6jc</t>
+        </is>
+      </c>
+      <c r="I480" t="n">
+        <v>1</v>
+      </c>
+      <c r="J480" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="K480" t="inlineStr">
+        <is>
+          <t>sexta-feira, 2 de fevereiro de 2024 18:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>R$ 29.620,00</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>GM - Chevrolet</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>Astra 2.0/ CD/ GLS 2.0 MPFI 16V 3p</t>
+        </is>
+      </c>
+      <c r="D481" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E481" t="inlineStr">
+        <is>
+          <t>Gasolina</t>
+        </is>
+      </c>
+      <c r="F481" t="inlineStr">
+        <is>
+          <t>004169-6</t>
+        </is>
+      </c>
+      <c r="G481" t="inlineStr">
+        <is>
+          <t xml:space="preserve">fevereiro de 2001 </t>
+        </is>
+      </c>
+      <c r="H481" t="inlineStr">
+        <is>
+          <t>pjmjmk4kqmc</t>
+        </is>
+      </c>
+      <c r="I481" t="n">
+        <v>1</v>
+      </c>
+      <c r="J481" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="K481" t="inlineStr">
+        <is>
+          <t>sexta-feira, 2 de fevereiro de 2024 18:08</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>